<commit_message>
TP#15469: Create new mapping for UK ETD tests
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK ETD.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK ETD.xlsx
@@ -186,9 +186,6 @@
     <t>ETD 3</t>
   </si>
   <si>
-    <t>INTERNATIONAL_EONOMY</t>
-  </si>
-  <si>
     <t>Intl Economy, Your Packaging</t>
   </si>
   <si>
@@ -519,6 +516,9 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL_ECONOMY</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1297,7 @@
   <dimension ref="A1:FM7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -1320,7 +1320,9 @@
     <col min="23" max="23" width="14.375" style="1" customWidth="1"/>
     <col min="24" max="31" width="9.125" style="1"/>
     <col min="32" max="32" width="32.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="88" width="9.125" style="1"/>
+    <col min="33" max="41" width="9.125" style="1"/>
+    <col min="42" max="42" width="23.375" style="1" customWidth="1"/>
+    <col min="43" max="88" width="9.125" style="1"/>
     <col min="89" max="89" width="14.125" style="1" customWidth="1"/>
     <col min="90" max="90" width="9.125" style="1"/>
     <col min="91" max="91" width="23" style="1" customWidth="1"/>
@@ -1329,277 +1331,277 @@
   <sheetData>
     <row r="1" spans="1:169" s="28" customFormat="1" ht="105.75" customHeight="1" thickBot="1">
       <c r="A1" s="36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F1" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="V1" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="W1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA1" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB1" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC1" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD1" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF1" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG1" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ1" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK1" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL1" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM1" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN1" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO1" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP1" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="AQ1" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="AR1" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="AS1" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT1" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="AV1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW1" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AX1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ1" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="BA1" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB1" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="BC1" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD1" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="BE1" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="BF1" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG1" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH1" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BK1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BL1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BM1" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="BN1" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="BO1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BP1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BQ1" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="BR1" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="BS1" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="BT1" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="BU1" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="BV1" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="BW1" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="BX1" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="BY1" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="BZ1" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="CA1" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="CB1" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="U1" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="V1" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="W1" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="X1" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y1" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z1" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA1" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB1" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="AC1" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="AD1" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE1" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF1" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="AG1" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH1" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI1" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="AJ1" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="AK1" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="AL1" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM1" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="AN1" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO1" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="AP1" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="AQ1" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="AR1" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="AS1" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="AT1" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="AU1" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="AV1" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="AW1" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="AX1" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="AY1" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="AZ1" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="BA1" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="BB1" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="BC1" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="BD1" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="BE1" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="BF1" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="BG1" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="BH1" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="BI1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BJ1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BK1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BL1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BM1" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="BN1" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="BO1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BP1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BQ1" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="BR1" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="BS1" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="BT1" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="BU1" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="BV1" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="BW1" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="BX1" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="BY1" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="BZ1" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="CA1" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="CB1" s="31" t="s">
-        <v>125</v>
-      </c>
       <c r="CC1" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD1" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CE1" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF1" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="CG1" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="CH1" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="CI1" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="CJ1" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="CK1" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="CL1" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CM1" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CN1" s="30"/>
       <c r="CO1" s="30"/>
@@ -1621,270 +1623,270 @@
     <row r="2" spans="1:169" s="20" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A2" s="37"/>
       <c r="B2" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
       <c r="E2" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="W2" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH2" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI2" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK2" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL2" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="AN2" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO2" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP2" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ2" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU2" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG2" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH2" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI2" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ2" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="BK2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="BL2" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="BN2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="BO2" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP2" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="BQ2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="BS2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="BT2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="BU2" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="BV2" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW2" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX2" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="BY2" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BZ2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="CA2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="CB2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="CC2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="CD2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="CE2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="CF2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="CG2" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="CH2" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="CI2" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="CJ2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="CK2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="CL2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="T2" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="U2" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="X2" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y2" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z2" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA2" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG2" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH2" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI2" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ2" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="AK2" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL2" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO2" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP2" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ2" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="AR2" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS2" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="AT2" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU2" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV2" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="AW2" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="BA2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="BB2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="BC2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="BD2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="BF2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="BH2" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="BI2" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="BJ2" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="BK2" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="BL2" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="BM2" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="BN2" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="BO2" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="BP2" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="BQ2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="BS2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="BT2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU2" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="BV2" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="BW2" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="BX2" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="BY2" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="BZ2" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="CA2" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="CB2" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="CC2" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="CD2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="CE2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="CF2" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="CG2" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="CH2" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="CI2" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="CJ2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="CK2" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="CL2" s="23" t="s">
-        <v>61</v>
-      </c>
       <c r="CM2" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="CN2" s="21"/>
       <c r="CO2" s="21"/>
@@ -1967,25 +1969,25 @@
     </row>
     <row r="3" spans="1:169" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A3" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>37</v>
@@ -2003,7 +2005,7 @@
         <v>35</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>33</v>
@@ -2300,19 +2302,19 @@
       </c>
       <c r="B4" s="40"/>
       <c r="C4" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>37</v>
@@ -2330,7 +2332,7 @@
         <v>35</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>33</v>
@@ -2627,11 +2629,11 @@
     </row>
     <row r="5" spans="1:169" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A5" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>40</v>
@@ -2643,7 +2645,7 @@
         <v>39</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
TP#20088: Defaulted just for physical print to false so that all tests run by default.  Fixed dangerous goods manipulator.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK ETD.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK ETD.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_lu1">#REF!</definedName>
     <definedName name="_lu2">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -493,9 +493,6 @@
     <t>ETD 3</t>
   </si>
   <si>
-    <t>INTERNATIONAL_EONOMY</t>
-  </si>
-  <si>
     <t>Intl Economy Freight, Box</t>
   </si>
   <si>
@@ -515,6 +512,9 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL_ECONOMY</t>
   </si>
 </sst>
 </file>
@@ -2124,8 +2124,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:FN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2150,7 +2150,7 @@
   <sheetData>
     <row r="1" spans="1:170" s="8" customFormat="1" ht="32.1" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
@@ -3473,7 +3473,7 @@
         <v>89</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>71</v>
@@ -3789,13 +3789,13 @@
       <c r="B6" s="48"/>
       <c r="C6" s="28"/>
       <c r="D6" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>70</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>89</v>
@@ -3819,7 +3819,7 @@
         <v>73</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O6" s="31" t="s">
         <v>120</v>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="Z6" s="31"/>
       <c r="AA6" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB6" s="31" t="s">
         <v>132</v>
@@ -4119,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="37" t="s">
@@ -4129,7 +4129,7 @@
         <v>70</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>89</v>
@@ -4153,7 +4153,7 @@
         <v>73</v>
       </c>
       <c r="N7" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O7" s="39" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
TP#20444: Fixed address where street number had no space after it.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK ETD.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK ETD.xlsx
@@ -478,9 +478,6 @@
     <t>ETD 1</t>
   </si>
   <si>
-    <t>1751tHOMPSON ST</t>
-  </si>
-  <si>
     <t>Intl Priority Freight, Box</t>
   </si>
   <si>
@@ -515,6 +512,9 @@
   </si>
   <si>
     <t>INTERNATIONAL_ECONOMY</t>
+  </si>
+  <si>
+    <t>1751 THOMPSON ST</t>
   </si>
 </sst>
 </file>
@@ -2124,8 +2124,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:FN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2140,7 +2140,7 @@
     <col min="8" max="8" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.140625" style="1" customWidth="1"/>
     <col min="10" max="23" width="9.140625" style="1"/>
-    <col min="24" max="24" width="14.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="32" width="9.140625" style="1"/>
     <col min="33" max="33" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="46" width="9.140625" style="1"/>
@@ -2150,7 +2150,7 @@
   <sheetData>
     <row r="1" spans="1:170" s="8" customFormat="1" ht="32.1" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
@@ -2861,7 +2861,7 @@
         <v>413104</v>
       </c>
       <c r="X3" s="25" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="Y3" s="22" t="s">
         <v>133</v>
@@ -3129,13 +3129,13 @@
       <c r="B4" s="47"/>
       <c r="C4" s="19"/>
       <c r="D4" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>70</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>89</v>
@@ -3159,7 +3159,7 @@
         <v>73</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O4" s="22" t="s">
         <v>120</v>
@@ -3192,7 +3192,7 @@
         <v>109</v>
       </c>
       <c r="Y4" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z4" s="22"/>
       <c r="AA4" s="22">
@@ -3467,13 +3467,13 @@
         <v>70</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>89</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>71</v>
@@ -3491,7 +3491,7 @@
         <v>73</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O5" s="22" t="s">
         <v>120</v>
@@ -3521,7 +3521,7 @@
         <v>413104</v>
       </c>
       <c r="X5" s="25" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="Y5" s="22" t="s">
         <v>133</v>
@@ -3789,13 +3789,13 @@
       <c r="B6" s="48"/>
       <c r="C6" s="28"/>
       <c r="D6" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>70</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>89</v>
@@ -3819,7 +3819,7 @@
         <v>73</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O6" s="31" t="s">
         <v>120</v>
@@ -3852,11 +3852,11 @@
         <v>109</v>
       </c>
       <c r="Y6" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z6" s="31"/>
       <c r="AA6" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AB6" s="31" t="s">
         <v>132</v>
@@ -4119,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="37" t="s">
@@ -4129,7 +4129,7 @@
         <v>70</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>89</v>
@@ -4153,7 +4153,7 @@
         <v>73</v>
       </c>
       <c r="N7" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O7" s="39" t="s">
         <v>120</v>
@@ -4183,7 +4183,7 @@
         <v>413140</v>
       </c>
       <c r="X7" s="42" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="Y7" s="39" t="s">
         <v>133</v>

</xml_diff>